<commit_message>
added demo script for running new project struture. Updated spreadsheet.  Added function to run national cascade.
</commit_message>
<xml_diff>
--- a/project_spreadsheets/test_national_project.xlsx
+++ b/project_spreadsheets/test_national_project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-34820" yWindow="20" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="-37280" yWindow="-2040" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>project name</t>
   </si>
@@ -90,7 +90,10 @@
     <t>values</t>
   </si>
   <si>
-    <t>Oct2016</t>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2016Oct</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -565,7 +568,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -573,7 +576,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -587,6 +590,9 @@
     <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>